<commit_message>
Comparison of Programs (continued)
</commit_message>
<xml_diff>
--- a/Process Documents/Comparison Degree Programs.xlsx
+++ b/Process Documents/Comparison Degree Programs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liafl\Dropbox\MSc Business Information Systems\Digitalisation of Business Processes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liafl\Documents\GitHub\digibp-monterosa\Process Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="36">
   <si>
     <t>Indicators</t>
   </si>
@@ -77,9 +77,6 @@
     <t>interest in international cultures</t>
   </si>
   <si>
-    <t>Skills Match</t>
-  </si>
-  <si>
     <t>Mathematics, logic thinking</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Marketing, Communication</t>
   </si>
   <si>
-    <t>Accounting, Auditing</t>
-  </si>
-  <si>
     <t>Business Analytics, Business Intelligence</t>
   </si>
   <si>
@@ -129,6 +123,15 @@
   </si>
   <si>
     <t>International Organizations</t>
+  </si>
+  <si>
+    <t>Skills/Interest Match</t>
+  </si>
+  <si>
+    <t>Accounting, Financial Auditing</t>
+  </si>
+  <si>
+    <t>Swiss Organization</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,7 +550,7 @@
     <row r="2" spans="1:6" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -651,12 +655,12 @@
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -676,7 +680,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -696,7 +700,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -716,7 +720,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -736,7 +740,7 @@
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -761,7 +765,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -781,7 +785,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -801,47 +805,187 @@
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>